<commit_message>
added evaluations for each models for the paper rebuttal
</commit_message>
<xml_diff>
--- a/JPS_Chatbot/Evaluation_results.xlsx
+++ b/JPS_Chatbot/Evaluation_results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xz378\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TWA2\TheWorldAvatar\JPS_Chatbot\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -3772,8 +3772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E118" sqref="E118"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added evaluation result compared with other KGQA systems
</commit_message>
<xml_diff>
--- a/JPS_Chatbot/Evaluation_results.xlsx
+++ b/JPS_Chatbot/Evaluation_results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15750" windowHeight="21300" firstSheet="2" activeTab="2"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="15750" windowHeight="21300" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="raw_data_1" sheetId="1" state="hidden" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2013" uniqueCount="535">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2012" uniqueCount="534">
   <si>
     <t>Question</t>
   </si>
@@ -1148,9 +1148,6 @@
     <t>enthalpy of fusion for tantalum nitride, mercuric sulfate, tungsten boride</t>
   </si>
   <si>
-    <t>Search for properties of an inorganic chemical class:</t>
-  </si>
-  <si>
     <t>oxides by refractive index</t>
   </si>
   <si>
@@ -1418,9 +1415,6 @@
     <t>homo lumo gap of methane</t>
   </si>
   <si>
-    <t>Possible molecules with weight 2000 g/mol</t>
-  </si>
-  <si>
     <t>Are molecules Benzodioxan and 3-Hydroxyacetophenone structurally similar</t>
   </si>
   <si>
@@ -1638,6 +1632,9 @@
   </si>
   <si>
     <t>what mechanism contains O + CH -&gt; H + CO</t>
+  </si>
+  <si>
+    <t>Possible molecules with weight over 2000 g/mol</t>
   </si>
 </sst>
 </file>
@@ -3772,18 +3769,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A114" sqref="A114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="70.140625" customWidth="1"/>
+    <col min="1" max="1" width="96.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="B1" t="s">
         <v>6</v>
@@ -3803,7 +3800,7 @@
     </row>
     <row r="2" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -3863,7 +3860,7 @@
     </row>
     <row r="5" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
@@ -3883,7 +3880,7 @@
     </row>
     <row r="6" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
@@ -3903,7 +3900,7 @@
     </row>
     <row r="7" spans="1:6" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
@@ -3913,12 +3910,12 @@
     </row>
     <row r="9" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -3933,7 +3930,7 @@
     </row>
     <row r="13" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -3943,17 +3940,17 @@
     </row>
     <row r="15" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
@@ -3978,42 +3975,42 @@
     </row>
     <row r="22" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="26" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="29" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="30" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
@@ -4023,7 +4020,7 @@
     </row>
     <row r="31" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="32" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
@@ -4033,7 +4030,7 @@
     </row>
     <row r="33" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="34" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
@@ -4048,37 +4045,37 @@
     </row>
     <row r="36" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="37" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="38" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="39" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="40" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="41" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="42" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="43" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
@@ -4093,7 +4090,7 @@
     </row>
     <row r="45" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="46" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
@@ -4108,32 +4105,32 @@
     </row>
     <row r="48" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>461</v>
+        <v>533</v>
       </c>
     </row>
     <row r="49" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
     </row>
     <row r="50" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="51" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="52" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="53" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="54" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
@@ -4178,7 +4175,7 @@
     </row>
     <row r="62" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="63" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
@@ -4198,17 +4195,17 @@
     </row>
     <row r="66" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="67" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="68" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="69" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
@@ -4233,12 +4230,12 @@
     </row>
     <row r="73" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="74" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="75" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
@@ -4268,7 +4265,7 @@
     </row>
     <row r="80" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="81" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
@@ -4308,12 +4305,12 @@
     </row>
     <row r="88" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="89" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="90" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
@@ -4323,12 +4320,12 @@
     </row>
     <row r="91" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
     </row>
     <row r="92" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="93" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
@@ -4338,7 +4335,7 @@
     </row>
     <row r="94" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="95" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
@@ -4348,7 +4345,7 @@
     </row>
     <row r="96" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="97" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
@@ -4368,12 +4365,12 @@
     </row>
     <row r="100" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="101" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="102" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
@@ -4388,7 +4385,7 @@
     </row>
     <row r="104" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="105" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
@@ -4408,37 +4405,37 @@
     </row>
     <row r="108" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
     </row>
     <row r="109" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="110" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="111" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="112" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="113" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="114" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
   </sheetData>
@@ -4454,8 +4451,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B224"/>
   <sheetViews>
-    <sheetView topLeftCell="A202" workbookViewId="0">
-      <selection activeCell="A225" sqref="A225"/>
+    <sheetView topLeftCell="A175" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A230" sqref="A230"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4463,89 +4460,110 @@
     <col min="1" max="1" width="77.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+        <v>423</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+        <v>421</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>346</v>
       </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
@@ -4580,7 +4598,7 @@
     </row>
     <row r="24" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
@@ -4590,22 +4608,22 @@
     </row>
     <row r="26" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="29" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="30" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
@@ -4620,7 +4638,7 @@
     </row>
     <row r="32" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
@@ -4630,18 +4648,18 @@
     </row>
     <row r="34" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B34" s="1"/>
     </row>
     <row r="35" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
@@ -4671,7 +4689,7 @@
     </row>
     <row r="42" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
@@ -4691,7 +4709,7 @@
     </row>
     <row r="46" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
@@ -4706,17 +4724,17 @@
     </row>
     <row r="49" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="50" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="51" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="52" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
@@ -4726,12 +4744,12 @@
     </row>
     <row r="53" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="54" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="55" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
@@ -4741,7 +4759,7 @@
     </row>
     <row r="56" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="57" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
@@ -4751,7 +4769,7 @@
     </row>
     <row r="58" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="59" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
@@ -4761,12 +4779,12 @@
     </row>
     <row r="60" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="61" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="62" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
@@ -4791,7 +4809,7 @@
     </row>
     <row r="66" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="67" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
@@ -4816,7 +4834,7 @@
     </row>
     <row r="71" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="72" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
@@ -4836,7 +4854,7 @@
     </row>
     <row r="75" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="76" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
@@ -4846,7 +4864,7 @@
     </row>
     <row r="77" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="78" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
@@ -4866,23 +4884,23 @@
     </row>
     <row r="81" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B82" s="1"/>
     </row>
     <row r="83" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
@@ -4902,22 +4920,22 @@
     </row>
     <row r="88" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
@@ -4927,7 +4945,7 @@
     </row>
     <row r="93" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
@@ -4937,32 +4955,32 @@
     </row>
     <row r="95" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="97" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="98" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="99" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="100" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="101" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
@@ -4972,23 +4990,21 @@
     </row>
     <row r="102" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="103" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="104" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="105" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A105" s="1" t="s">
-        <v>371</v>
-      </c>
+      <c r="A105" s="1"/>
     </row>
     <row r="106" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
@@ -4997,12 +5013,12 @@
     </row>
     <row r="107" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="108" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="109" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
@@ -5072,12 +5088,12 @@
     </row>
     <row r="122" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="123" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="124" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
@@ -5097,17 +5113,17 @@
     </row>
     <row r="127" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="128" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="129" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="130" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
@@ -5122,7 +5138,7 @@
     </row>
     <row r="132" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="133" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
@@ -5162,7 +5178,7 @@
     </row>
     <row r="140" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="141" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
@@ -5258,7 +5274,7 @@
     </row>
     <row r="159" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B159" s="1"/>
     </row>
@@ -5300,7 +5316,7 @@
     </row>
     <row r="167" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="168" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
@@ -5368,7 +5384,7 @@
     </row>
     <row r="180" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="181" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
@@ -5383,7 +5399,7 @@
     </row>
     <row r="183" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="184" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
@@ -5418,7 +5434,7 @@
     </row>
     <row r="190" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="191" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
@@ -5464,7 +5480,7 @@
     </row>
     <row r="199" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="200" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
@@ -5511,89 +5527,89 @@
     </row>
     <row r="208" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="209" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B209" s="1"/>
     </row>
     <row r="210" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="211" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A211" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="212" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B212" s="1"/>
     </row>
     <row r="213" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="214" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A214" s="1" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="215" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="216" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="217" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A217" s="1" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="218" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="219" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A219" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="220" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A220" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="221" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A221" s="1" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="222" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A222" s="1" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="223" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="224" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A224" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
   </sheetData>
@@ -5610,13 +5626,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F98"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="A99" sqref="A99"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="79.28515625" customWidth="1"/>
+    <col min="1" max="1" width="118" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -5741,7 +5757,7 @@
     </row>
     <row r="7" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
@@ -5801,7 +5817,7 @@
     </row>
     <row r="10" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="B10" t="s">
         <v>5</v>
@@ -5921,7 +5937,7 @@
     </row>
     <row r="16" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="B16" t="s">
         <v>5</v>
@@ -6301,7 +6317,7 @@
     </row>
     <row r="35" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="B35" t="s">
         <v>5</v>
@@ -6436,7 +6452,7 @@
     </row>
     <row r="44" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -6551,7 +6567,7 @@
     </row>
     <row r="67" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="68" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
@@ -6571,7 +6587,7 @@
     </row>
     <row r="71" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="72" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
@@ -6616,7 +6632,7 @@
     </row>
     <row r="80" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
     </row>
     <row r="81" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
@@ -6676,37 +6692,37 @@
     </row>
     <row r="92" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="93" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="94" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
     </row>
     <row r="95" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="96" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
     </row>
     <row r="97" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="98" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
   </sheetData>
@@ -6722,8 +6738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F89"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A62" sqref="A62"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="F59" sqref="F59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6734,27 +6750,12 @@
   <sheetData>
     <row r="1" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
+        <v>204</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>105</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -6769,132 +6770,42 @@
         <v>5</v>
       </c>
       <c r="F2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" t="s">
-        <v>14</v>
+        <v>522</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" t="s">
-        <v>14</v>
+        <v>210</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" t="s">
-        <v>14</v>
+        <v>272</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F6" t="s">
-        <v>14</v>
+        <v>524</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" t="s">
-        <v>5</v>
-      </c>
-      <c r="F7" t="s">
-        <v>14</v>
+        <v>243</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F8" t="s">
-        <v>23</v>
+        <v>232</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
@@ -6914,99 +6825,39 @@
     </row>
     <row r="10" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" t="s">
-        <v>5</v>
-      </c>
-      <c r="F10" t="s">
-        <v>14</v>
+        <v>202</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E11" t="s">
-        <v>5</v>
-      </c>
-      <c r="F11" t="s">
-        <v>14</v>
+        <v>203</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" t="s">
-        <v>5</v>
-      </c>
-      <c r="F12" t="s">
-        <v>14</v>
+        <v>520</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" t="s">
-        <v>5</v>
-      </c>
-      <c r="E13" t="s">
-        <v>5</v>
-      </c>
-      <c r="F13" t="s">
-        <v>14</v>
+        <v>209</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>48</v>
+        <v>108</v>
       </c>
       <c r="B14" t="s">
         <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D14" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E14" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F14" t="s">
         <v>14</v>
@@ -7014,33 +6865,18 @@
     </row>
     <row r="15" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" t="s">
-        <v>5</v>
-      </c>
-      <c r="E15" t="s">
-        <v>5</v>
-      </c>
-      <c r="F15" t="s">
-        <v>14</v>
+        <v>211</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="B16" t="s">
         <v>5</v>
       </c>
       <c r="C16" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D16" t="s">
         <v>5</v>
@@ -7054,287 +6890,77 @@
     </row>
     <row r="17" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" t="s">
-        <v>6</v>
-      </c>
-      <c r="E17" t="s">
-        <v>5</v>
-      </c>
-      <c r="F17" t="s">
-        <v>14</v>
+        <v>233</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" t="s">
-        <v>5</v>
-      </c>
-      <c r="E18" t="s">
-        <v>5</v>
-      </c>
-      <c r="F18" t="s">
-        <v>14</v>
+        <v>221</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B19" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" t="s">
-        <v>6</v>
-      </c>
-      <c r="E19" t="s">
-        <v>5</v>
-      </c>
-      <c r="F19" t="s">
-        <v>14</v>
+        <v>234</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B20" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" t="s">
-        <v>5</v>
-      </c>
-      <c r="E20" t="s">
-        <v>5</v>
-      </c>
-      <c r="F20" t="s">
-        <v>14</v>
+        <v>525</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B21" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" t="s">
-        <v>5</v>
-      </c>
-      <c r="E21" t="s">
-        <v>5</v>
-      </c>
-      <c r="F21" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B22" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" t="s">
-        <v>5</v>
-      </c>
-      <c r="D22" t="s">
-        <v>5</v>
-      </c>
-      <c r="E22" t="s">
-        <v>5</v>
-      </c>
-      <c r="F22" t="s">
-        <v>14</v>
+        <v>130</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B23" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23" t="s">
-        <v>5</v>
-      </c>
-      <c r="E23" t="s">
-        <v>5</v>
-      </c>
-      <c r="F23" t="s">
-        <v>14</v>
+        <v>129</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B24" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" t="s">
-        <v>5</v>
-      </c>
-      <c r="E24" t="s">
-        <v>5</v>
-      </c>
-      <c r="F24" t="s">
-        <v>14</v>
+        <v>521</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B25" t="s">
-        <v>5</v>
-      </c>
-      <c r="C25" t="s">
-        <v>5</v>
-      </c>
-      <c r="D25" t="s">
-        <v>5</v>
-      </c>
-      <c r="E25" t="s">
-        <v>5</v>
-      </c>
-      <c r="F25" t="s">
-        <v>14</v>
+        <v>223</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B26" t="s">
-        <v>5</v>
-      </c>
-      <c r="C26" t="s">
-        <v>5</v>
-      </c>
-      <c r="D26" t="s">
-        <v>5</v>
-      </c>
-      <c r="E26" t="s">
-        <v>5</v>
-      </c>
-      <c r="F26" t="s">
-        <v>14</v>
+        <v>225</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B27" t="s">
-        <v>5</v>
-      </c>
-      <c r="C27" t="s">
-        <v>5</v>
-      </c>
-      <c r="D27" t="s">
-        <v>81</v>
-      </c>
-      <c r="E27" t="s">
-        <v>5</v>
-      </c>
-      <c r="F27" t="s">
-        <v>14</v>
+        <v>219</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B28" t="s">
-        <v>5</v>
-      </c>
-      <c r="C28" t="s">
-        <v>5</v>
-      </c>
-      <c r="D28" t="s">
-        <v>6</v>
-      </c>
-      <c r="E28" t="s">
-        <v>5</v>
-      </c>
-      <c r="F28" t="s">
-        <v>14</v>
+        <v>519</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B29" t="s">
-        <v>5</v>
-      </c>
-      <c r="C29" t="s">
-        <v>5</v>
-      </c>
-      <c r="D29" t="s">
-        <v>5</v>
-      </c>
-      <c r="E29" t="s">
-        <v>5</v>
-      </c>
-      <c r="F29" t="s">
-        <v>14</v>
+        <v>253</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B30" t="s">
-        <v>5</v>
-      </c>
-      <c r="C30" t="s">
-        <v>5</v>
-      </c>
-      <c r="D30" t="s">
-        <v>5</v>
-      </c>
-      <c r="E30" t="s">
-        <v>5</v>
-      </c>
-      <c r="F30" t="s">
-        <v>14</v>
+        <v>222</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>89</v>
+        <v>22</v>
       </c>
       <c r="B31" t="s">
         <v>5</v>
@@ -7343,7 +6969,7 @@
         <v>5</v>
       </c>
       <c r="D31" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E31" t="s">
         <v>5</v>
@@ -7354,27 +6980,12 @@
     </row>
     <row r="32" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B32" t="s">
-        <v>5</v>
-      </c>
-      <c r="C32" t="s">
-        <v>5</v>
-      </c>
-      <c r="D32" t="s">
-        <v>5</v>
-      </c>
-      <c r="E32" t="s">
-        <v>5</v>
-      </c>
-      <c r="F32" t="s">
-        <v>14</v>
+        <v>277</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>105</v>
+        <v>86</v>
       </c>
       <c r="B33" t="s">
         <v>5</v>
@@ -7383,7 +6994,7 @@
         <v>5</v>
       </c>
       <c r="D33" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E33" t="s">
         <v>5</v>
@@ -7394,19 +7005,19 @@
     </row>
     <row r="34" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>108</v>
+        <v>71</v>
       </c>
       <c r="B34" t="s">
         <v>5</v>
       </c>
       <c r="C34" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D34" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E34" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F34" t="s">
         <v>14</v>
@@ -7414,249 +7025,624 @@
     </row>
     <row r="35" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B35" t="s">
-        <v>5</v>
-      </c>
-      <c r="C35" t="s">
-        <v>5</v>
-      </c>
-      <c r="D35" t="s">
-        <v>6</v>
-      </c>
-      <c r="E35" t="s">
-        <v>5</v>
-      </c>
-      <c r="F35" t="s">
-        <v>14</v>
+        <v>127</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>124</v>
+        <v>19</v>
+      </c>
+      <c r="B36" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36" t="s">
+        <v>6</v>
+      </c>
+      <c r="E36" t="s">
+        <v>5</v>
+      </c>
+      <c r="F36" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>127</v>
+        <v>273</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>129</v>
+        <v>49</v>
+      </c>
+      <c r="B38" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38" t="s">
+        <v>5</v>
+      </c>
+      <c r="E38" t="s">
+        <v>5</v>
+      </c>
+      <c r="F38" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>130</v>
+        <v>527</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>209</v>
+        <v>231</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>210</v>
+        <v>48</v>
+      </c>
+      <c r="B41" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41" t="s">
+        <v>5</v>
+      </c>
+      <c r="D41" t="s">
+        <v>5</v>
+      </c>
+      <c r="E41" t="s">
+        <v>5</v>
+      </c>
+      <c r="F41" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>211</v>
+        <v>528</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>219</v>
+        <v>95</v>
+      </c>
+      <c r="B43" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" t="s">
+        <v>6</v>
+      </c>
+      <c r="E43" t="s">
+        <v>6</v>
+      </c>
+      <c r="F43" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>221</v>
+        <v>46</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>222</v>
+        <v>137</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>225</v>
+        <v>73</v>
+      </c>
+      <c r="B47" t="s">
+        <v>5</v>
+      </c>
+      <c r="C47" t="s">
+        <v>6</v>
+      </c>
+      <c r="D47" t="s">
+        <v>5</v>
+      </c>
+      <c r="E47" t="s">
+        <v>5</v>
+      </c>
+      <c r="F47" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+      <c r="B48" t="s">
+        <v>5</v>
+      </c>
+      <c r="C48" t="s">
+        <v>6</v>
+      </c>
+      <c r="D48" t="s">
+        <v>5</v>
+      </c>
+      <c r="E48" t="s">
+        <v>5</v>
+      </c>
+      <c r="F48" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="B49" t="s">
+        <v>5</v>
+      </c>
+      <c r="C49" t="s">
+        <v>5</v>
+      </c>
+      <c r="D49" t="s">
+        <v>6</v>
+      </c>
+      <c r="E49" t="s">
+        <v>5</v>
+      </c>
+      <c r="F49" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="B50" t="s">
+        <v>5</v>
+      </c>
+      <c r="C50" t="s">
+        <v>5</v>
+      </c>
+      <c r="D50" t="s">
+        <v>6</v>
+      </c>
+      <c r="E50" t="s">
+        <v>5</v>
+      </c>
+      <c r="F50" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="B51" t="s">
+        <v>5</v>
+      </c>
+      <c r="C51" t="s">
+        <v>5</v>
+      </c>
+      <c r="D51" t="s">
+        <v>5</v>
+      </c>
+      <c r="E51" t="s">
+        <v>5</v>
+      </c>
+      <c r="F51" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+      <c r="B52" t="s">
+        <v>5</v>
+      </c>
+      <c r="C52" t="s">
+        <v>5</v>
+      </c>
+      <c r="D52" t="s">
+        <v>5</v>
+      </c>
+      <c r="E52" t="s">
+        <v>5</v>
+      </c>
+      <c r="F52" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+      <c r="B53" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53" t="s">
+        <v>5</v>
+      </c>
+      <c r="D53" t="s">
+        <v>6</v>
+      </c>
+      <c r="E53" t="s">
+        <v>5</v>
+      </c>
+      <c r="F53" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+      <c r="B55" t="s">
+        <v>5</v>
+      </c>
+      <c r="C55" t="s">
+        <v>5</v>
+      </c>
+      <c r="D55" t="s">
+        <v>5</v>
+      </c>
+      <c r="E55" t="s">
+        <v>5</v>
+      </c>
+      <c r="F55" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="B56" t="s">
+        <v>5</v>
+      </c>
+      <c r="C56" t="s">
+        <v>5</v>
+      </c>
+      <c r="D56" t="s">
+        <v>6</v>
+      </c>
+      <c r="E56" t="s">
+        <v>5</v>
+      </c>
+      <c r="F56" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="B58" t="s">
+        <v>5</v>
+      </c>
+      <c r="C58" t="s">
+        <v>5</v>
+      </c>
+      <c r="D58" t="s">
+        <v>6</v>
+      </c>
+      <c r="E58" t="s">
+        <v>5</v>
+      </c>
+      <c r="F58" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="B59" t="s">
+        <v>5</v>
+      </c>
+      <c r="C59" t="s">
+        <v>6</v>
+      </c>
+      <c r="D59" t="s">
+        <v>5</v>
+      </c>
+      <c r="E59" t="s">
+        <v>5</v>
+      </c>
+      <c r="F59" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="B60" t="s">
+        <v>5</v>
+      </c>
+      <c r="C60" t="s">
+        <v>5</v>
+      </c>
+      <c r="D60" t="s">
+        <v>6</v>
+      </c>
+      <c r="E60" t="s">
+        <v>5</v>
+      </c>
+      <c r="F60" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="B63" t="s">
+        <v>5</v>
+      </c>
+      <c r="C63" t="s">
+        <v>5</v>
+      </c>
+      <c r="D63" t="s">
+        <v>5</v>
+      </c>
+      <c r="E63" t="s">
+        <v>5</v>
+      </c>
+      <c r="F63" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>277</v>
+        <v>20</v>
+      </c>
+      <c r="B64" t="s">
+        <v>5</v>
+      </c>
+      <c r="C64" t="s">
+        <v>5</v>
+      </c>
+      <c r="D64" t="s">
+        <v>6</v>
+      </c>
+      <c r="E64" t="s">
+        <v>5</v>
+      </c>
+      <c r="F64" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>278</v>
+        <v>47</v>
+      </c>
+      <c r="B65" t="s">
+        <v>5</v>
+      </c>
+      <c r="C65" t="s">
+        <v>5</v>
+      </c>
+      <c r="D65" t="s">
+        <v>5</v>
+      </c>
+      <c r="E65" t="s">
+        <v>5</v>
+      </c>
+      <c r="F65" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>279</v>
+        <v>18</v>
+      </c>
+      <c r="B66" t="s">
+        <v>5</v>
+      </c>
+      <c r="C66" t="s">
+        <v>5</v>
+      </c>
+      <c r="D66" t="s">
+        <v>6</v>
+      </c>
+      <c r="E66" t="s">
+        <v>5</v>
+      </c>
+      <c r="F66" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>29</v>
+        <v>89</v>
+      </c>
+      <c r="B67" t="s">
+        <v>5</v>
+      </c>
+      <c r="C67" t="s">
+        <v>5</v>
+      </c>
+      <c r="D67" t="s">
+        <v>5</v>
+      </c>
+      <c r="E67" t="s">
+        <v>5</v>
+      </c>
+      <c r="F67" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>30</v>
+        <v>124</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
+      </c>
+      <c r="B69" t="s">
+        <v>5</v>
+      </c>
+      <c r="C69" t="s">
+        <v>5</v>
+      </c>
+      <c r="D69" t="s">
+        <v>6</v>
+      </c>
+      <c r="E69" t="s">
+        <v>5</v>
+      </c>
+      <c r="F69" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>32</v>
+        <v>276</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>34</v>
+        <v>40</v>
+      </c>
+      <c r="B71" t="s">
+        <v>5</v>
+      </c>
+      <c r="C71" t="s">
+        <v>6</v>
+      </c>
+      <c r="D71" t="s">
+        <v>5</v>
+      </c>
+      <c r="E71" t="s">
+        <v>5</v>
+      </c>
+      <c r="F71" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>46</v>
+        <v>70</v>
+      </c>
+      <c r="B72" t="s">
+        <v>5</v>
+      </c>
+      <c r="C72" t="s">
+        <v>5</v>
+      </c>
+      <c r="D72" t="s">
+        <v>5</v>
+      </c>
+      <c r="E72" t="s">
+        <v>5</v>
+      </c>
+      <c r="F72" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>128</v>
+        <v>229</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>137</v>
+        <v>244</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>202</v>
+        <v>69</v>
+      </c>
+      <c r="B75" t="s">
+        <v>5</v>
+      </c>
+      <c r="C75" t="s">
+        <v>6</v>
+      </c>
+      <c r="D75" t="s">
+        <v>5</v>
+      </c>
+      <c r="E75" t="s">
+        <v>5</v>
+      </c>
+      <c r="F75" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>203</v>
+        <v>75</v>
+      </c>
+      <c r="B76" t="s">
+        <v>5</v>
+      </c>
+      <c r="C76" t="s">
+        <v>5</v>
+      </c>
+      <c r="D76" t="s">
+        <v>5</v>
+      </c>
+      <c r="E76" t="s">
+        <v>5</v>
+      </c>
+      <c r="F76" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="77" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>204</v>
+        <v>251</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>85</v>
+        <v>21</v>
       </c>
       <c r="B78" t="s">
         <v>5</v>
       </c>
       <c r="C78" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D78" t="s">
         <v>6</v>
       </c>
       <c r="E78" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F78" t="s">
         <v>14</v>
@@ -7664,75 +7650,108 @@
     </row>
     <row r="79" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B79" t="s">
-        <v>5</v>
-      </c>
-      <c r="C79" t="s">
-        <v>6</v>
-      </c>
-      <c r="D79" t="s">
-        <v>6</v>
-      </c>
-      <c r="E79" t="s">
-        <v>6</v>
-      </c>
-      <c r="F79" t="s">
-        <v>14</v>
+        <v>275</v>
       </c>
     </row>
     <row r="80" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B84" t="s">
+        <v>5</v>
+      </c>
+      <c r="C84" t="s">
+        <v>5</v>
+      </c>
+      <c r="D84" t="s">
+        <v>6</v>
+      </c>
+      <c r="E84" t="s">
+        <v>5</v>
+      </c>
+      <c r="F84" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="83" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="88" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="B87" t="s">
+        <v>5</v>
+      </c>
+      <c r="C87" t="s">
+        <v>5</v>
+      </c>
+      <c r="D87" t="s">
+        <v>81</v>
+      </c>
+      <c r="E87" t="s">
+        <v>5</v>
+      </c>
+      <c r="F87" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="89" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>530</v>
+        <v>85</v>
+      </c>
+      <c r="B89" t="s">
+        <v>5</v>
+      </c>
+      <c r="C89" t="s">
+        <v>6</v>
+      </c>
+      <c r="D89" t="s">
+        <v>6</v>
+      </c>
+      <c r="E89" t="s">
+        <v>6</v>
+      </c>
+      <c r="F89" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A1:F89">
+    <sortCondition ref="A1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>